<commit_message>
Stark MOP bill importer
</commit_message>
<xml_diff>
--- a/test/electricity/bills.mop.stark.xlsx
+++ b/test/electricity/bills.mop.stark.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="HH" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t xml:space="preserve">Invoice Date</t>
   </si>
@@ -171,23 +172,47 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B6:I12"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.2091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.51530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.26020408163265"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.4081632653061"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="10.4591836734694"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.01020408163265"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.98469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B6:I13"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="5.66836734693878"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.75"/>
   </cols>
   <sheetData>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -247,6 +272,32 @@
         <v>704.3</v>
       </c>
       <c r="I12" s="0" t="n">
+        <v>135.81</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="3" t="n">
+        <v>1472066139971</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="4" t="n">
+        <v>29738</v>
+      </c>
+      <c r="G13" s="4" t="n">
+        <v>29767</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>704.3</v>
+      </c>
+      <c r="I13" s="0" t="n">
         <v>135.81</v>
       </c>
     </row>

</xml_diff>